<commit_message>
Up next announcement lijnde te hoog uit sinds introductie verticaal centreren.
</commit_message>
<xml_diff>
--- a/Package/Config_Interfaces/Landmarks_Categories.xlsx
+++ b/Package/Config_Interfaces/Landmarks_Categories.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Landmarks" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="186">
   <si>
     <t>A</t>
   </si>
@@ -60,18 +60,12 @@
     <t>#wetenschap #studenten</t>
   </si>
   <si>
-    <t>P, W, H</t>
-  </si>
-  <si>
     <t>#fictie #boeken #verhalen #reizen #bibliotheek</t>
   </si>
   <si>
     <t>#fictie #boeken #lezen</t>
   </si>
   <si>
-    <t>P, R, V, W, H</t>
-  </si>
-  <si>
     <t>bibliotheek</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>#treinstation #straat #drukte</t>
   </si>
   <si>
-    <t>P, R, H</t>
-  </si>
-  <si>
     <t>park</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>#park #lente #gras</t>
   </si>
   <si>
-    <t>R, I, H</t>
-  </si>
-  <si>
     <t>theater achterom</t>
   </si>
   <si>
@@ -108,9 +96,6 @@
     <t>#theater #kunst #humor #verhalen #inspireren</t>
   </si>
   <si>
-    <t>I, V, H</t>
-  </si>
-  <si>
     <t>kerkstraat</t>
   </si>
   <si>
@@ -120,9 +105,6 @@
     <t>#straat #stad</t>
   </si>
   <si>
-    <t>R, H</t>
-  </si>
-  <si>
     <t>Heb jij vanochtend gezongen onder de douche?</t>
   </si>
   <si>
@@ -588,10 +570,22 @@
     <t>C</t>
   </si>
   <si>
+    <t>P, H</t>
+  </si>
+  <si>
+    <t>W, H</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V, H</t>
+  </si>
+  <si>
+    <t>A, H</t>
+  </si>
+  <si>
+    <t>I, H</t>
+  </si>
+  <si>
     <t>humor</t>
-  </si>
-  <si>
-    <t>Wat zullen we er eens over zeggen?</t>
   </si>
 </sst>
 </file>
@@ -640,8 +634,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -664,7 +680,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -674,6 +690,17 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -683,6 +710,17 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -980,7 +1018,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -991,72 +1029,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1071,401 +1109,443 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>179</v>
       </c>
       <c r="D1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" t="s">
-        <v>184</v>
-      </c>
-      <c r="D19" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
-      </c>
-      <c r="D20" t="s">
-        <v>183</v>
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>179</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="D24" t="s">
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
-      </c>
-      <c r="D25" t="s">
-        <v>183</v>
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>178</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" t="s">
-        <v>185</v>
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>177</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D27" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -1473,13 +1553,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -1490,16 +1570,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D29" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -1507,425 +1587,416 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>185</v>
-      </c>
-      <c r="D30" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D32" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" t="s">
-        <v>184</v>
-      </c>
-      <c r="D33" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>185</v>
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>179</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D37" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>185</v>
-      </c>
-      <c r="D41" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D43" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D44" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D45" t="s">
+        <v>177</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>185</v>
+        <v>178</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D47" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D48" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="D49" t="s">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="D51" t="s">
+        <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>179</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D53" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D54" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>184</v>
-      </c>
-      <c r="D55" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="D56" t="s">
+        <v>0</v>
       </c>
       <c r="E56" t="s">
         <v>3</v>
@@ -1933,1109 +2004,1073 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C57" t="s">
+        <v>178</v>
       </c>
       <c r="E57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
-      </c>
-      <c r="C58" t="s">
-        <v>185</v>
-      </c>
-      <c r="D58" t="s">
-        <v>183</v>
+        <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D59" t="s">
+        <v>177</v>
       </c>
       <c r="E59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D60" t="s">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>178</v>
       </c>
       <c r="E60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C61" t="s">
+        <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
-      </c>
-      <c r="D62" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="E62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
-      </c>
-      <c r="C63" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64" t="s">
-        <v>183</v>
+        <v>16</v>
       </c>
       <c r="E64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
-      </c>
-      <c r="D65" t="s">
-        <v>183</v>
+        <v>16</v>
+      </c>
+      <c r="C65" t="s">
+        <v>179</v>
       </c>
       <c r="E65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>185</v>
+        <v>178</v>
+      </c>
+      <c r="D67" t="s">
+        <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
-      </c>
-      <c r="C69" t="s">
-        <v>184</v>
-      </c>
-      <c r="D69" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D70" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D72" t="s">
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D73" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
-        <v>19</v>
-      </c>
-      <c r="C74" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
-        <v>19</v>
-      </c>
-      <c r="D75" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D76" t="s">
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C77" t="s">
-        <v>184</v>
-      </c>
-      <c r="D77" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="E77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
-        <v>19</v>
-      </c>
-      <c r="C78" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="D78" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E78" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
-      </c>
-      <c r="C79" t="s">
-        <v>185</v>
-      </c>
-      <c r="D79" t="s">
-        <v>183</v>
+        <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="B80" t="s">
         <v>19</v>
       </c>
-      <c r="C80" t="s">
-        <v>184</v>
-      </c>
       <c r="D80" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E80" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
-      <c r="C81" t="s">
-        <v>185</v>
+      <c r="D81" t="s">
+        <v>177</v>
       </c>
       <c r="E81" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D82" t="s">
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
-      </c>
-      <c r="C83" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D83" t="s">
+        <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D84" t="s">
+        <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B85" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D85" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E85" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B86" t="s">
-        <v>23</v>
-      </c>
-      <c r="C86" t="s">
-        <v>184</v>
+        <v>19</v>
       </c>
       <c r="E86" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E87" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E88" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C89" t="s">
+        <v>179</v>
       </c>
       <c r="D89" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E89" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>178</v>
       </c>
       <c r="E90" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="D91" t="s">
+        <v>177</v>
       </c>
       <c r="E91" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D92" t="s">
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D93" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E93" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="D94" t="s">
+        <v>177</v>
       </c>
       <c r="E94" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E95" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D96" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E96" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="B97" t="s">
-        <v>23</v>
-      </c>
-      <c r="D97" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E97" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D98" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E98" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B99" t="s">
-        <v>23</v>
-      </c>
-      <c r="C99" t="s">
-        <v>184</v>
-      </c>
-      <c r="D99" t="s">
-        <v>183</v>
+        <v>19</v>
       </c>
       <c r="E99" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C100" t="s">
+        <v>178</v>
       </c>
       <c r="D100" t="s">
         <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D101" t="s">
+        <v>177</v>
       </c>
       <c r="E101" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B102" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D102" t="s">
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="B103" t="s">
-        <v>23</v>
-      </c>
-      <c r="C103" t="s">
-        <v>185</v>
+        <v>19</v>
+      </c>
+      <c r="D103" t="s">
+        <v>177</v>
       </c>
       <c r="E103" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="B104" t="s">
-        <v>23</v>
-      </c>
-      <c r="D104" t="s">
-        <v>183</v>
+        <v>19</v>
+      </c>
+      <c r="C104" t="s">
+        <v>179</v>
       </c>
       <c r="E104" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="B105" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="C105" t="s">
+        <v>178</v>
       </c>
       <c r="E105" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C106" t="s">
+        <v>179</v>
       </c>
       <c r="D106" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="B107" t="s">
-        <v>15</v>
-      </c>
-      <c r="D107" t="s">
-        <v>183</v>
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>178</v>
       </c>
       <c r="E107" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="B108" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D108" t="s">
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="B109" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C109" t="s">
+        <v>179</v>
       </c>
       <c r="D109" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E109" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E110" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B111" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>184</v>
-      </c>
-      <c r="D111" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E111" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="B112" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E112" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B113" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E113" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="B114" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="B115" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>185</v>
-      </c>
-      <c r="D115" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E115" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B116" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="D116" t="s">
+        <v>0</v>
       </c>
       <c r="E116" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B117" t="s">
-        <v>15</v>
-      </c>
-      <c r="C117" t="s">
-        <v>185</v>
-      </c>
-      <c r="D117" t="s">
-        <v>183</v>
+        <v>12</v>
       </c>
       <c r="E117" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B118" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D118" t="s">
         <v>0</v>
       </c>
       <c r="E118" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="B119" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D119" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E119" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B120" t="s">
-        <v>15</v>
-      </c>
-      <c r="C120" t="s">
-        <v>185</v>
-      </c>
-      <c r="D120" t="s">
-        <v>183</v>
+        <v>12</v>
       </c>
       <c r="E120" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B121" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C121" t="s">
+        <v>178</v>
       </c>
       <c r="E121" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>15</v>
-      </c>
-      <c r="C122" t="s">
-        <v>185</v>
+        <v>12</v>
       </c>
       <c r="D122" t="s">
-        <v>183</v>
+        <v>51</v>
       </c>
       <c r="E122" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="B123" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E123" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="B124" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" t="s">
-        <v>185</v>
-      </c>
-      <c r="D124" t="s">
-        <v>183</v>
+        <v>12</v>
       </c>
       <c r="E124" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B125" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C125" t="s">
+        <v>179</v>
+      </c>
+      <c r="D125" t="s">
+        <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="B126" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>184</v>
-      </c>
-      <c r="D126" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="E126" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B127" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C127" t="s">
+        <v>179</v>
       </c>
       <c r="D127" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E127" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B128" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C128" t="s">
-        <v>184</v>
-      </c>
-      <c r="D128" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="E128" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B129" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C129" t="s">
+        <v>179</v>
       </c>
       <c r="D129" t="s">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="E129" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="B130" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E130" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B131" t="s">
-        <v>7</v>
-      </c>
-      <c r="C131" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="E131" t="s">
         <v>6</v>
@@ -3043,16 +3078,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B132" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C132" t="s">
-        <v>185</v>
-      </c>
-      <c r="D132" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="E132" t="s">
         <v>6</v>
@@ -3060,13 +3092,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B133" t="s">
-        <v>7</v>
-      </c>
-      <c r="C133" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="E133" t="s">
         <v>6</v>
@@ -3074,16 +3103,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C134" t="s">
-        <v>185</v>
-      </c>
-      <c r="D134" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="E134" t="s">
         <v>6</v>
@@ -3091,371 +3117,740 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="B135" t="s">
-        <v>7</v>
-      </c>
-      <c r="C135" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="D135" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="D136" t="s">
+        <v>177</v>
       </c>
       <c r="E136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C137" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="D137" t="s">
+        <v>0</v>
       </c>
       <c r="E137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="D138" t="s">
+        <v>0</v>
       </c>
       <c r="E138" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="B139" t="s">
-        <v>7</v>
-      </c>
-      <c r="C139" t="s">
-        <v>184</v>
+        <v>22</v>
+      </c>
+      <c r="D139" t="s">
+        <v>0</v>
       </c>
       <c r="E139" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C140" t="s">
-        <v>185</v>
+        <v>178</v>
+      </c>
+      <c r="D140" t="s">
+        <v>177</v>
       </c>
       <c r="E140" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B141" t="s">
-        <v>7</v>
-      </c>
-      <c r="C141" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="E141" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="B142" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C142" t="s">
-        <v>184</v>
-      </c>
-      <c r="D142" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="E142" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B143" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C143" t="s">
+        <v>179</v>
       </c>
       <c r="E143" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C144" t="s">
+        <v>179</v>
       </c>
       <c r="D144" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E144" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B145" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C145" t="s">
-        <v>185</v>
-      </c>
-      <c r="D145" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="E145" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B146" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C146" t="s">
+        <v>179</v>
+      </c>
+      <c r="D146" t="s">
+        <v>177</v>
       </c>
       <c r="E146" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B147" t="s">
-        <v>7</v>
-      </c>
-      <c r="C147" t="s">
-        <v>184</v>
+        <v>22</v>
+      </c>
+      <c r="D147" t="s">
+        <v>0</v>
       </c>
       <c r="E147" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B148" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C148" t="s">
+        <v>179</v>
       </c>
       <c r="D148" t="s">
-        <v>57</v>
+        <v>177</v>
       </c>
       <c r="E148" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C149" t="s">
+        <v>179</v>
+      </c>
+      <c r="D149" t="s">
+        <v>177</v>
       </c>
       <c r="E149" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B150" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E150" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B151" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C151" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D151" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E151" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B152" t="s">
-        <v>7</v>
-      </c>
-      <c r="C152" t="s">
-        <v>184</v>
+        <v>22</v>
       </c>
       <c r="E152" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B153" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C153" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D153" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
       <c r="E153" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B154" t="s">
-        <v>7</v>
-      </c>
-      <c r="C154" t="s">
-        <v>184</v>
+        <v>22</v>
       </c>
       <c r="E154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B155" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C155" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D155" t="s">
         <v>0</v>
       </c>
       <c r="E155" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B156" t="s">
-        <v>7</v>
-      </c>
-      <c r="C156" t="s">
-        <v>184</v>
+        <v>22</v>
+      </c>
+      <c r="D156" t="s">
+        <v>177</v>
       </c>
       <c r="E156" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="B157" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C157" t="s">
+        <v>178</v>
+      </c>
+      <c r="D157" t="s">
+        <v>0</v>
       </c>
       <c r="E157" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B158" t="s">
-        <v>7</v>
-      </c>
-      <c r="C158" t="s">
-        <v>185</v>
+        <v>22</v>
+      </c>
+      <c r="D158" t="s">
+        <v>177</v>
       </c>
       <c r="E158" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B159" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C159" t="s">
+        <v>179</v>
       </c>
       <c r="E159" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="B160" t="s">
-        <v>7</v>
-      </c>
-      <c r="C160" t="s">
         <v>185</v>
       </c>
+      <c r="D160" t="s">
+        <v>177</v>
+      </c>
       <c r="E160" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>187</v>
+        <v>26</v>
       </c>
       <c r="B161" t="s">
+        <v>185</v>
+      </c>
+      <c r="E161" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>27</v>
       </c>
-      <c r="E161" t="s">
-        <v>6</v>
+      <c r="B162" t="s">
+        <v>185</v>
+      </c>
+      <c r="D162" t="s">
+        <v>177</v>
+      </c>
+      <c r="E162" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>28</v>
+      </c>
+      <c r="B163" t="s">
+        <v>185</v>
+      </c>
+      <c r="D163" t="s">
+        <v>177</v>
+      </c>
+      <c r="E163" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>29</v>
+      </c>
+      <c r="B164" t="s">
+        <v>185</v>
+      </c>
+      <c r="D164" t="s">
+        <v>177</v>
+      </c>
+      <c r="E164" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>30</v>
+      </c>
+      <c r="B165" t="s">
+        <v>185</v>
+      </c>
+      <c r="C165" t="s">
+        <v>178</v>
+      </c>
+      <c r="E165" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>31</v>
+      </c>
+      <c r="B166" t="s">
+        <v>185</v>
+      </c>
+      <c r="C166" t="s">
+        <v>179</v>
+      </c>
+      <c r="D166" t="s">
+        <v>0</v>
+      </c>
+      <c r="E166" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>32</v>
+      </c>
+      <c r="B167" t="s">
+        <v>185</v>
+      </c>
+      <c r="C167" t="s">
+        <v>179</v>
+      </c>
+      <c r="E167" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>33</v>
+      </c>
+      <c r="B168" t="s">
+        <v>185</v>
+      </c>
+      <c r="C168" t="s">
+        <v>178</v>
+      </c>
+      <c r="D168" t="s">
+        <v>0</v>
+      </c>
+      <c r="E168" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>34</v>
+      </c>
+      <c r="B169" t="s">
+        <v>185</v>
+      </c>
+      <c r="E169" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>35</v>
+      </c>
+      <c r="B170" t="s">
+        <v>185</v>
+      </c>
+      <c r="E170" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>36</v>
+      </c>
+      <c r="B171" t="s">
+        <v>185</v>
+      </c>
+      <c r="C171" t="s">
+        <v>179</v>
+      </c>
+      <c r="D171" t="s">
+        <v>177</v>
+      </c>
+      <c r="E171" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>37</v>
+      </c>
+      <c r="B172" t="s">
+        <v>185</v>
+      </c>
+      <c r="D172" t="s">
+        <v>0</v>
+      </c>
+      <c r="E172" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>38</v>
+      </c>
+      <c r="B173" t="s">
+        <v>185</v>
+      </c>
+      <c r="C173" t="s">
+        <v>178</v>
+      </c>
+      <c r="D173" t="s">
+        <v>0</v>
+      </c>
+      <c r="E173" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>39</v>
+      </c>
+      <c r="B174" t="s">
+        <v>185</v>
+      </c>
+      <c r="C174" t="s">
+        <v>179</v>
+      </c>
+      <c r="E174" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>40</v>
+      </c>
+      <c r="B175" t="s">
+        <v>185</v>
+      </c>
+      <c r="E175" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>41</v>
+      </c>
+      <c r="B176" t="s">
+        <v>185</v>
+      </c>
+      <c r="D176" t="s">
+        <v>0</v>
+      </c>
+      <c r="E176" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>42</v>
+      </c>
+      <c r="B177" t="s">
+        <v>185</v>
+      </c>
+      <c r="C177" t="s">
+        <v>179</v>
+      </c>
+      <c r="D177" t="s">
+        <v>177</v>
+      </c>
+      <c r="E177" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>43</v>
+      </c>
+      <c r="B178" t="s">
+        <v>185</v>
+      </c>
+      <c r="C178" t="s">
+        <v>178</v>
+      </c>
+      <c r="D178" t="s">
+        <v>0</v>
+      </c>
+      <c r="E178" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>44</v>
+      </c>
+      <c r="B179" t="s">
+        <v>185</v>
+      </c>
+      <c r="D179" t="s">
+        <v>177</v>
+      </c>
+      <c r="E179" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>45</v>
+      </c>
+      <c r="B180" t="s">
+        <v>185</v>
+      </c>
+      <c r="C180" t="s">
+        <v>178</v>
+      </c>
+      <c r="D180" t="s">
+        <v>0</v>
+      </c>
+      <c r="E180" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>46</v>
+      </c>
+      <c r="B181" t="s">
+        <v>185</v>
+      </c>
+      <c r="C181" t="s">
+        <v>179</v>
+      </c>
+      <c r="E181" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>47</v>
+      </c>
+      <c r="B182" t="s">
+        <v>185</v>
+      </c>
+      <c r="E182" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>48</v>
+      </c>
+      <c r="B183" t="s">
+        <v>185</v>
+      </c>
+      <c r="C183" t="s">
+        <v>179</v>
+      </c>
+      <c r="E183" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>49</v>
+      </c>
+      <c r="B184" t="s">
+        <v>185</v>
+      </c>
+      <c r="D184" t="s">
+        <v>177</v>
+      </c>
+      <c r="E184" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>50</v>
+      </c>
+      <c r="B185" t="s">
+        <v>185</v>
+      </c>
+      <c r="C185" t="s">
+        <v>179</v>
+      </c>
+      <c r="E185" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nieuwe content indeling Atossa
</commit_message>
<xml_diff>
--- a/Package/Config_Interfaces/Landmarks_Categories.xlsx
+++ b/Package/Config_Interfaces/Landmarks_Categories.xlsx
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135:XFD159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Inregeling hooks: geen "MS Word-style" quotes, die worden niet goed afgebeeld.
</commit_message>
<xml_diff>
--- a/Package/Config_Interfaces/Landmarks_Categories.xlsx
+++ b/Package/Config_Interfaces/Landmarks_Categories.xlsx
@@ -117,9 +117,6 @@
     <t>Ben je meer een ochtend- of een koffiepersoon?</t>
   </si>
   <si>
-    <t>Hoe vaak snooze jij ‘s ochtends de wekker?</t>
-  </si>
-  <si>
     <t>Wat is jouw vreemdste gewoonte?</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Het is onmogelijk voor mensen om te niezen met open ogen</t>
   </si>
   <si>
-    <t>Ga nu naar Google en toets het woord ‘askew’ in bij afbeeldingen, wat zie je?</t>
-  </si>
-  <si>
     <t>Hoe meer mogelijkheden je telefoon heeft, des te meer tijd je doorbrengt op het toilet</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>Voel jij je wel eens eenzaam?</t>
   </si>
   <si>
-    <t>Wist jij dat veel Nederlanders in de jaren 50’ klaar stonden om Oost-Europese vluchtelingen op te vangen?</t>
-  </si>
-  <si>
     <t>Hoe sta jij tegenover de toenemende migratiestroom?</t>
   </si>
   <si>
@@ -240,9 +231,6 @@
     <t>Heb jij er wel eens over nagedacht hoe het zou zijn als je van het andere geslacht was?</t>
   </si>
   <si>
-    <t>Wanneer was de laatste keer dat je ‘ik hou van jou’ zei?</t>
-  </si>
-  <si>
     <t>Denk jij dat de politiek de werkelijkheid uit het oog verliest?</t>
   </si>
   <si>
@@ -465,15 +453,9 @@
     <t>Laat je niet klein maken door een ander!</t>
   </si>
   <si>
-    <t>Je kan beter denken ‘ik kan niet geloven dat ik dit gedaan heb!’ in plaats van ‘ik wou dat ik dat gedaan had’</t>
-  </si>
-  <si>
     <t>Is je leeftijd slechts een getal?</t>
   </si>
   <si>
-    <t>Wanneer was de laatste keer dat je zei ‘ik hou van jou’?</t>
-  </si>
-  <si>
     <t>Ooit geprobeerd om iets te verschuiven met je gedachte?</t>
   </si>
   <si>
@@ -586,6 +568,24 @@
   </si>
   <si>
     <t>humor</t>
+  </si>
+  <si>
+    <t>Hoe vaak snooze jij 's ochtends de wekker?</t>
+  </si>
+  <si>
+    <t>Wist jij dat veel Nederlanders in de jaren 50' klaar stonden om Oost-Europese vluchtelingen op te vangen?</t>
+  </si>
+  <si>
+    <t>Wanneer was de laatste keer dat je 'ik hou van jou' zei?</t>
+  </si>
+  <si>
+    <t>Je kan beter denken 'ik kan niet geloven dat ik dit gedaan heb!' in plaats van 'ik wou dat ik dat gedaan had'</t>
+  </si>
+  <si>
+    <t>Wanneer was de laatste keer dat je zei 'ik hou van jou'?</t>
+  </si>
+  <si>
+    <t>Ga nu naar Google en toets het woord 'askew' in bij afbeeldingen, wat zie je?</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1018,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1032,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1046,7 +1046,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -1060,7 +1060,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -1074,7 +1074,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -1088,7 +1088,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A83" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,16 +1124,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1141,13 +1141,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1158,16 +1158,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -1175,13 +1175,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1206,13 +1206,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1223,13 +1223,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1240,13 +1240,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -1268,13 +1268,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1282,13 +1282,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1299,13 +1299,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1316,16 +1316,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -1333,13 +1333,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -1367,13 +1367,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -1381,16 +1381,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
@@ -1398,16 +1398,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>182</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
@@ -1440,13 +1440,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
@@ -1457,13 +1457,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -1491,16 +1491,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
@@ -1522,13 +1522,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -1536,13 +1536,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -1553,13 +1553,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -1570,16 +1570,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D29" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -1587,13 +1587,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
         <v>3</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1615,16 +1615,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D32" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
@@ -1685,16 +1685,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E37" t="s">
         <v>3</v>
@@ -1702,13 +1702,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -1716,13 +1716,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1744,13 +1744,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
@@ -1758,13 +1758,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
         <v>3</v>
@@ -1772,13 +1772,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D43" t="s">
         <v>0</v>
@@ -1789,13 +1789,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D44" t="s">
         <v>0</v>
@@ -1806,16 +1806,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
         <v>0</v>
@@ -1840,16 +1840,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D47" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
@@ -1857,16 +1857,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -1888,13 +1888,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D50" t="s">
         <v>0</v>
@@ -1905,13 +1905,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
         <v>0</v>
@@ -1922,16 +1922,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -1939,16 +1939,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D53" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -1956,16 +1956,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -1973,13 +1973,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -1987,13 +1987,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
         <v>0</v>
@@ -2004,13 +2004,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
         <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E57" t="s">
         <v>2</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B58" t="s">
         <v>16</v>
@@ -2029,16 +2029,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B59" t="s">
         <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D59" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
         <v>2</v>
@@ -2046,13 +2046,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
         <v>16</v>
       </c>
       <c r="C60" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
         <v>2</v>
@@ -2060,13 +2060,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
         <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E61" t="s">
         <v>2</v>
@@ -2074,13 +2074,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
         <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
         <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E63" t="s">
         <v>2</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
         <v>16</v>
@@ -2113,13 +2113,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
         <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E65" t="s">
         <v>2</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
         <v>16</v>
@@ -2141,13 +2141,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
         <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D67" t="s">
         <v>0</v>
@@ -2158,13 +2158,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B68" t="s">
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E68" t="s">
         <v>2</v>
@@ -2172,7 +2172,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
         <v>16</v>
@@ -2183,16 +2183,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
         <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D70" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E70" t="s">
         <v>2</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
         <v>16</v>
@@ -2214,13 +2214,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
         <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D72" t="s">
         <v>0</v>
@@ -2231,16 +2231,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B73" t="s">
         <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D73" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E73" t="s">
         <v>2</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
         <v>16</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
         <v>16</v>
@@ -2273,13 +2273,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
         <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D76" t="s">
         <v>0</v>
@@ -2290,13 +2290,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
         <v>16</v>
       </c>
       <c r="C77" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E77" t="s">
         <v>2</v>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
       </c>
       <c r="D78" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E78" t="s">
         <v>2</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
@@ -2335,7 +2335,7 @@
         <v>19</v>
       </c>
       <c r="D80" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E80" t="s">
         <v>5</v>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="D81" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E81" t="s">
         <v>5</v>
@@ -2357,13 +2357,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B82" t="s">
         <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D82" t="s">
         <v>0</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B83" t="s">
         <v>19</v>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
         <v>19</v>
@@ -2402,16 +2402,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B85" t="s">
         <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D85" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E85" t="s">
         <v>5</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
         <v>19</v>
@@ -2430,13 +2430,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B87" t="s">
         <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E87" t="s">
         <v>5</v>
@@ -2444,13 +2444,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B88" t="s">
         <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E88" t="s">
         <v>5</v>
@@ -2458,16 +2458,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B89" t="s">
         <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D89" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E89" t="s">
         <v>5</v>
@@ -2475,13 +2475,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B90" t="s">
         <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E90" t="s">
         <v>5</v>
@@ -2489,16 +2489,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B91" t="s">
         <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D91" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E91" t="s">
         <v>5</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B92" t="s">
         <v>19</v>
@@ -2520,16 +2520,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B93" t="s">
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D93" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E93" t="s">
         <v>5</v>
@@ -2537,16 +2537,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B94" t="s">
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D94" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E94" t="s">
         <v>5</v>
@@ -2554,7 +2554,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B95" t="s">
         <v>19</v>
@@ -2565,16 +2565,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B96" t="s">
         <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D96" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E96" t="s">
         <v>5</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
         <v>19</v>
@@ -2593,16 +2593,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B98" t="s">
         <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D98" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E98" t="s">
         <v>5</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B99" t="s">
         <v>19</v>
@@ -2621,13 +2621,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B100" t="s">
         <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D100" t="s">
         <v>0</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B101" t="s">
         <v>19</v>
       </c>
       <c r="D101" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E101" t="s">
         <v>5</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D102" t="s">
         <v>0</v>
@@ -2669,13 +2669,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B103" t="s">
         <v>19</v>
       </c>
       <c r="D103" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E103" t="s">
         <v>5</v>
@@ -2683,13 +2683,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="B104" t="s">
         <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E104" t="s">
         <v>5</v>
@@ -2697,13 +2697,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B105" t="s">
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E105" t="s">
         <v>6</v>
@@ -2711,13 +2711,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D106" t="s">
         <v>0</v>
@@ -2728,13 +2728,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E107" t="s">
         <v>6</v>
@@ -2742,13 +2742,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D108" t="s">
         <v>0</v>
@@ -2759,16 +2759,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D109" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E109" t="s">
         <v>6</v>
@@ -2776,7 +2776,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
@@ -2787,13 +2787,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B111" t="s">
         <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E111" t="s">
         <v>6</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
@@ -2812,13 +2812,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B113" t="s">
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E113" t="s">
         <v>6</v>
@@ -2826,13 +2826,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E114" t="s">
         <v>6</v>
@@ -2840,13 +2840,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E115" t="s">
         <v>6</v>
@@ -2854,13 +2854,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D116" t="s">
         <v>0</v>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B117" t="s">
         <v>12</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B118" t="s">
         <v>12</v>
@@ -2896,13 +2896,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B119" t="s">
         <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D119" t="s">
         <v>0</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -2924,13 +2924,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B121" t="s">
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E121" t="s">
         <v>6</v>
@@ -2938,13 +2938,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B122" t="s">
         <v>12</v>
       </c>
       <c r="D122" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E122" t="s">
         <v>6</v>
@@ -2952,7 +2952,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B123" t="s">
         <v>12</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B124" t="s">
         <v>12</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B125" t="s">
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D125" t="s">
         <v>0</v>
@@ -2991,13 +2991,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B126" t="s">
         <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E126" t="s">
         <v>6</v>
@@ -3005,13 +3005,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B127" t="s">
         <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D127" t="s">
         <v>0</v>
@@ -3022,13 +3022,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
         <v>12</v>
       </c>
       <c r="C128" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E128" t="s">
         <v>6</v>
@@ -3036,13 +3036,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B129" t="s">
         <v>12</v>
       </c>
       <c r="C129" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D129" t="s">
         <v>0</v>
@@ -3053,13 +3053,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E130" t="s">
         <v>6</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B131" t="s">
         <v>12</v>
@@ -3078,13 +3078,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
       </c>
       <c r="C132" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E132" t="s">
         <v>6</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B133" t="s">
         <v>12</v>
@@ -3103,13 +3103,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B134" t="s">
         <v>12</v>
       </c>
       <c r="C134" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E134" t="s">
         <v>6</v>
@@ -3123,7 +3123,7 @@
         <v>22</v>
       </c>
       <c r="D135" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E135" t="s">
         <v>5</v>
@@ -3131,13 +3131,13 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B136" t="s">
         <v>22</v>
       </c>
       <c r="D136" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E136" t="s">
         <v>5</v>
@@ -3145,13 +3145,13 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B137" t="s">
         <v>22</v>
       </c>
       <c r="C137" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D137" t="s">
         <v>0</v>
@@ -3162,7 +3162,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B138" t="s">
         <v>22</v>
@@ -3176,7 +3176,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B139" t="s">
         <v>22</v>
@@ -3190,16 +3190,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B140" t="s">
         <v>22</v>
       </c>
       <c r="C140" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D140" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E140" t="s">
         <v>5</v>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B141" t="s">
         <v>22</v>
@@ -3218,13 +3218,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B142" t="s">
         <v>22</v>
       </c>
       <c r="C142" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E142" t="s">
         <v>5</v>
@@ -3232,13 +3232,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B143" t="s">
         <v>22</v>
       </c>
       <c r="C143" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E143" t="s">
         <v>5</v>
@@ -3246,16 +3246,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B144" t="s">
         <v>22</v>
       </c>
       <c r="C144" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D144" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E144" t="s">
         <v>5</v>
@@ -3263,13 +3263,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B145" t="s">
         <v>22</v>
       </c>
       <c r="C145" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E145" t="s">
         <v>5</v>
@@ -3277,16 +3277,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B146" t="s">
         <v>22</v>
       </c>
       <c r="C146" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D146" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E146" t="s">
         <v>5</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B147" t="s">
         <v>22</v>
@@ -3308,16 +3308,16 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B148" t="s">
         <v>22</v>
       </c>
       <c r="C148" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D148" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E148" t="s">
         <v>5</v>
@@ -3325,16 +3325,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B149" t="s">
         <v>22</v>
       </c>
       <c r="C149" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D149" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E149" t="s">
         <v>5</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B150" t="s">
         <v>22</v>
@@ -3353,16 +3353,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B151" t="s">
         <v>22</v>
       </c>
       <c r="C151" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D151" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E151" t="s">
         <v>5</v>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B152" t="s">
         <v>22</v>
@@ -3381,16 +3381,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B153" t="s">
         <v>22</v>
       </c>
       <c r="C153" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D153" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E153" t="s">
         <v>5</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B154" t="s">
         <v>22</v>
@@ -3409,13 +3409,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B155" t="s">
         <v>22</v>
       </c>
       <c r="C155" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D155" t="s">
         <v>0</v>
@@ -3426,13 +3426,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B156" t="s">
         <v>22</v>
       </c>
       <c r="D156" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E156" t="s">
         <v>5</v>
@@ -3440,13 +3440,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="B157" t="s">
         <v>22</v>
       </c>
       <c r="C157" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D157" t="s">
         <v>0</v>
@@ -3457,13 +3457,13 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B158" t="s">
         <v>22</v>
       </c>
       <c r="D158" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E158" t="s">
         <v>5</v>
@@ -3471,13 +3471,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="B159" t="s">
         <v>22</v>
       </c>
       <c r="C159" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E159" t="s">
         <v>5</v>
@@ -3488,10 +3488,10 @@
         <v>25</v>
       </c>
       <c r="B160" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D160" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E160" t="s">
         <v>1</v>
@@ -3502,7 +3502,7 @@
         <v>26</v>
       </c>
       <c r="B161" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E161" t="s">
         <v>1</v>
@@ -3513,10 +3513,10 @@
         <v>27</v>
       </c>
       <c r="B162" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D162" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E162" t="s">
         <v>1</v>
@@ -3527,10 +3527,10 @@
         <v>28</v>
       </c>
       <c r="B163" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D163" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E163" t="s">
         <v>1</v>
@@ -3538,13 +3538,13 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>29</v>
+        <v>180</v>
       </c>
       <c r="B164" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D164" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E164" t="s">
         <v>1</v>
@@ -3552,13 +3552,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B165" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C165" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E165" t="s">
         <v>1</v>
@@ -3566,13 +3566,13 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B166" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C166" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D166" t="s">
         <v>0</v>
@@ -3583,13 +3583,13 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B167" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C167" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E167" t="s">
         <v>1</v>
@@ -3597,13 +3597,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B168" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C168" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D168" t="s">
         <v>0</v>
@@ -3614,10 +3614,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B169" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E169" t="s">
         <v>1</v>
@@ -3625,10 +3625,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B170" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E170" t="s">
         <v>1</v>
@@ -3636,16 +3636,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B171" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C171" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D171" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E171" t="s">
         <v>1</v>
@@ -3653,10 +3653,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B172" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D172" t="s">
         <v>0</v>
@@ -3667,13 +3667,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B173" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C173" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D173" t="s">
         <v>0</v>
@@ -3684,13 +3684,13 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B174" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C174" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E174" t="s">
         <v>1</v>
@@ -3698,10 +3698,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B175" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E175" t="s">
         <v>1</v>
@@ -3709,10 +3709,10 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B176" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D176" t="s">
         <v>0</v>
@@ -3723,16 +3723,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B177" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C177" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D177" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E177" t="s">
         <v>1</v>
@@ -3740,13 +3740,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B178" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C178" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D178" t="s">
         <v>0</v>
@@ -3757,13 +3757,13 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B179" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D179" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E179" t="s">
         <v>1</v>
@@ -3771,13 +3771,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B180" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C180" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D180" t="s">
         <v>0</v>
@@ -3788,13 +3788,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="B181" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C181" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E181" t="s">
         <v>1</v>
@@ -3802,10 +3802,10 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B182" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E182" t="s">
         <v>1</v>
@@ -3813,13 +3813,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B183" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C183" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E183" t="s">
         <v>1</v>
@@ -3827,13 +3827,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B184" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D184" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E184" t="s">
         <v>1</v>
@@ -3841,13 +3841,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B185" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C185" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E185" t="s">
         <v>1</v>

</xml_diff>